<commit_message>
Code made to select the most frequently returned trial per patient and return any unique trials
</commit_message>
<xml_diff>
--- a/SMC Challenge 6/eligibility criteria/Dataset1_Hemoglobin_Trials_First.xlsx
+++ b/SMC Challenge 6/eligibility criteria/Dataset1_Hemoglobin_Trials_First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\ClinicalTrialChallenge\SMC Challenge 6\eligibility criteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E009B1-618D-4877-B736-483F2A5E4090}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDFF8B7-6C58-4995-9C8C-D684873B52FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3568,10 +3568,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G348"/>
+  <dimension ref="A1:H348"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G131" sqref="G131"/>
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -5989,7 +5989,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>234</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>237</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="226.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="226.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>241</v>
       </c>
@@ -6054,11 +6054,11 @@
       <c r="F131" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="G131" s="5" t="s">
+      <c r="H131" s="5" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>244</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="61.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="61.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>784</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="61.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="61.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>787</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="46.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="46.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>790</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>248</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="106.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="106.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>793</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>251</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>255</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="46.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="46.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>796</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>258</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>262</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="31.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="31.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>799</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="144" spans="1:7" s="5" customFormat="1" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" s="5" customFormat="1" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>265</v>
       </c>

</xml_diff>